<commit_message>
re-run results for the addiction submission
</commit_message>
<xml_diff>
--- a/templates/results_template_final.xlsx
+++ b/templates/results_template_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitLab\SPECTRUM\Projects\smoke-free-dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10612A13-C961-4E08-B2CA-B0C17BB73654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473F6E6A-50C3-4533-94E5-718BEAB0E705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="7" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="121">
   <si>
     <t>All</t>
   </si>
@@ -379,16 +379,31 @@
     <t>(5) Total excise % of price</t>
   </si>
   <si>
-    <t>(6) Total legal HRT spend (£m)</t>
-  </si>
-  <si>
-    <t>(7) Total illicit HRT spend (£m)</t>
-  </si>
-  <si>
     <t>Factory-Made Cigarettes</t>
   </si>
   <si>
     <t>Hand-Rolled Tobacco</t>
+  </si>
+  <si>
+    <t>(1) Total duty receipts (£bn)</t>
+  </si>
+  <si>
+    <t>(6) Total legal HRT spend (£bn)</t>
+  </si>
+  <si>
+    <t>(7) Total illicit HRT spend (£bn)</t>
+  </si>
+  <si>
+    <t>(9) Total legal cigarette spend (£bn)</t>
+  </si>
+  <si>
+    <t>(10) Total illicit cigarette spend (£bn)</t>
+  </si>
+  <si>
+    <t>Totals (£bn)</t>
+  </si>
+  <si>
+    <t>Table S1. Breakdown of the Upshift Calculation</t>
   </si>
 </sst>
 </file>
@@ -712,6 +727,19 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -727,32 +755,19 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,27 +1103,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60" t="s">
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
       <c r="H3" s="13" t="s">
         <v>36</v>
       </c>
@@ -1248,15 +1263,15 @@
       <c r="H14" s="27"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1324,22 +1339,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="61" t="s">
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="63" t="s">
+      <c r="G1" s="70"/>
+      <c r="H1" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -5758,12 +5773,12 @@
       <c r="E1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -7655,12 +7670,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
@@ -12875,62 +12890,67 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:H18"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70" t="s">
-        <v>36</v>
+      <c r="B2" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="60" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="73">
-        <f>'Upshift Calcs'!D4</f>
+        <v>114</v>
+      </c>
+      <c r="D4" s="64">
+        <f>'Upshift Calcs'!D4/1000</f>
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="73">
-        <f>'Upshift Calcs'!G4</f>
+        <v>114</v>
+      </c>
+      <c r="G4" s="64">
+        <f>'Upshift Calcs'!G4/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -12938,21 +12958,20 @@
       <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="63">
         <f>'Upshift Calcs'!D5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="71"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="67">
         <f>'Upshift Calcs'!D6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -12961,14 +12980,14 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="32">
         <f>'Upshift Calcs'!D7</f>
         <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="73">
+      <c r="G7" s="63">
         <f>'Upshift Calcs'!G7</f>
         <v>0</v>
       </c>
@@ -12977,14 +12996,14 @@
       <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="63">
         <f>'Upshift Calcs'!D8</f>
         <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
       </c>
-      <c r="G8" s="73">
+      <c r="G8" s="63">
         <f>'Upshift Calcs'!G8</f>
         <v>0</v>
       </c>
@@ -12996,7 +13015,7 @@
       <c r="C9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D9" s="77">
         <f>'Upshift Calcs'!D9</f>
         <v>0</v>
       </c>
@@ -13006,7 +13025,7 @@
       <c r="F9" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="32">
         <f>'Upshift Calcs'!G9</f>
         <v>0</v>
       </c>
@@ -13018,7 +13037,7 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="32">
         <f>'Upshift Calcs'!D10</f>
         <v>0</v>
       </c>
@@ -13030,7 +13049,7 @@
       <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="18">
         <f>'Upshift Calcs'!D11</f>
         <v>0</v>
       </c>
@@ -13040,83 +13059,91 @@
       <c r="F11" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="18">
         <f>'Upshift Calcs'!G11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="65">
-        <f>'Upshift Calcs'!D12</f>
+      <c r="D12" s="43">
+        <f>'Upshift Calcs'!D12/1000</f>
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F12" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="65">
-        <f>'Upshift Calcs'!G12</f>
+      <c r="G12" s="43">
+        <f>'Upshift Calcs'!G12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="43">
+        <f>'Upshift Calcs'!H12/1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="65">
-        <f>'Upshift Calcs'!D13</f>
+        <v>118</v>
+      </c>
+      <c r="D13" s="43">
+        <f>'Upshift Calcs'!D13/1000</f>
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" s="65">
-        <f>'Upshift Calcs'!G13</f>
+        <v>116</v>
+      </c>
+      <c r="G13" s="43">
+        <f>'Upshift Calcs'!G13/1000</f>
         <v>0</v>
       </c>
+      <c r="H13" s="43">
+        <f>'Upshift Calcs'!H13/1000</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H14" s="76">
-        <f>'Upshift Calcs'!H14</f>
+      <c r="H14" s="65">
+        <f>'Upshift Calcs'!H14/1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
     </row>
     <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="75"/>
-      <c r="H16" s="77">
-        <f>'Upshift Calcs'!H16</f>
+      <c r="G16" s="61"/>
+      <c r="H16" s="66">
+        <f>'Upshift Calcs'!H16/1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="68">
-        <f>'Upshift Calcs'!C18</f>
+      <c r="C18" s="62">
+        <f>'Upshift Calcs'!C19</f>
         <v>0</v>
       </c>
       <c r="D18" s="29"/>
@@ -13162,8 +13189,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
       <c r="C2" s="34" t="s">
         <v>72</v>
       </c>

</xml_diff>